<commit_message>
Split dataset for finetuning
</commit_message>
<xml_diff>
--- a/data/test/relevancy-test-5768.xlsx
+++ b/data/test/relevancy-test-5768.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,27 +448,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>You do have on the website a page and email address to accept public comments and requests regarding the Federal Power Act section 202 but I just want to make sure that they will be posted for the public to see</t>
+          <t>S 389 extends the existing credit and creates a second drilling window that also applies to heavy oil</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Federal Power Act requires FERC to balance those competing interests in issuing a license because no one use of a river for power drinking water irrigation recreation or other use should automatically take precedence</t>
+          <t>However while we look forward to advanced nuclear technology development it is long overdue to solve our Nations nuclear waste disposal challenge</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>In 2000 these nuclear power plants produced a record 755 thousand gigawatthours of electricity</t>
+          <t>By definition costeffective conservation is less costly than any other energy resource and conservation reduces consumers bills</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,37 +478,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>They include the bioremediation of mixed waste at many of the contaminated DOE sites the witchs brew that we have left from the legacy of cold war also the enhanced sequestration of carbon by the terrestrial and marine biosphere in order to reduce the atmospheric concentrations of greenhouse gases in the atmosphere and also as has already been mentioned the production of clean fuels such as hydrogen through the miracles of biotechnology</t>
+          <t>They have no electricity</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mr Barrett under the Nuclear Waste Policy Act we gave Nevada the tools which really means the money they need to oppose the Yucca licensing process at the NRC</t>
+          <t>And I hope that we can find new ways to use coal even cleaner than we are using it today</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Renewable diesel that lowers agricultural emissions is fully compatible with existing diesel assets and has a place at the table too</t>
+          <t>Electricity generation demand is largely a function of weather heat in the west and cold in the east</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Our nations comprehensive energy policy must ensure an affordable reliable supply of energy and nuclear energy provides one of the solutions to several policy challenges that our nation faces</t>
+          <t>Last year the House included a provision in its energy bill requiring a Federal study into this boutique motor fuel issue</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -518,17 +518,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ultimately advanced concepts such as that of the DOEs Vision 21 program offer the advantages of clean efficient power with simultaneous production of liquid transportation fuels to reduce our dependence on imported petroleum</t>
+          <t>Do we have any planes that can fly on electricity plugin hybrid technology</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>FERC grid operators State public utility commissions and power plants even progressive power companies are already planning for the changes that are under way</t>
+          <t>Likewise when insurance companies are able to pull their market power to negotiate lower rates there can be positive results</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -538,87 +538,87 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>As you know Mr Chairman there have been many developments in the Nations energy portfolio since FERC issued Order No</t>
+          <t>Our work on energy issues has described some of the consequences of hurricanes on petroleum marketssuch as rapid gasoline price increases</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>This group spent over two years evaluating and documenting best practices from across all types of energy pipeline systems</t>
+          <t>The technology allows older coal plants to be retrofitted to burn cleaner eliminating the hassle of permitting a new power plant</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>The job creators the haulers the steel mills have all lost the ability to create jobs because of a policy that was designed and I will just end on this a policy that was designed to protect us against state oil interests</t>
+          <t>CAFE standards have helped increase the average fuel economy of our lightduty vehicle fleet</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>So is the EPA do you have the statutory authority are you considering relaxing the ethanol mandate due to the corn shortage</t>
+          <t>There were no septic systems no water systems and they ended up drilling their own wells and they become really a problem</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A mere requestsomehow provide some assistance so they could be an existing power plant and have beenhave been rebuffed</t>
+          <t>We are committed to working with Congress to explore ways to maintain or enhance environmental benefits of clean fuels programs while exploring ways to increase the flexibility of the fuels distribution infrastructure and minimize costs</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Nuclear Waste Policy Act of 1982 made the transportation and longterm storage of nuclear waste the responsibility of the Secretary of Energy</t>
+          <t>This simply reflects the large amount of capital necessary to find refine and distribute petroleum products</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Electricity generation demand is largely a function of weather heat in the west and cold in the east</t>
+          <t>There is a great controversy right now Congressman over the Environmental Protection Agencys proposed rules for particulate emissions from coal plants and also greenhouse gas emissions</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>There is no question that the oxygenate ability of ethanol is a positive</t>
+          <t>The Maryland Energy Assistance Program which distributes LIHEAP funds locally is expected to receive 32 million from the Federal Government</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>To highlight a few first we should reestablish and expand Federal agency targets for annual improvements and energy efficiency renewable energy and other key metrics and make needed changes to unlock the use of contracting mechanisms that leverage private funds for public efficiency and renewable projects</t>
+          <t>I am pleased to present the administrations views on the need for comprehensive energy legislation</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -628,7 +628,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>There is a great deal of uncertainty about the size and availability of crude oil resources particularly conventional resources the adequacy of investment capital and geopolitical trends</t>
+          <t>We greatly appreciate the bipartisan support for coal in the Committee as reflected in both the Housepassed version of HR</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -638,7 +638,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>But we do have an oil crisis</t>
+          <t>Well that was under the greenhouse gas requirement but did anyone at EPA consult with the Office of Management and Budget or the White House before moving forward with taking over the flexible permitting program under the Clean Air Act</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -648,17 +648,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Estimated potential energy savings expected to result when this program is fully implemented are in the 35 range</t>
+          <t>We had great debate over whether this administration the Obama administration is hostile to energy production on land offshore and on Federal lands etc and the argument that that is the case is not supported by the facts</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>In terms of the policies of Alberta there are policies in place to recognize that the upfront costs of developing oil sands are very very high</t>
+          <t>Emissions markets are established early and can provide accurate price signals to all involved</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -668,27 +668,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>This one is from TXU Energy down in Texas</t>
+          <t>fuel receipt and the transportation systems to be compatible with the currently NRC licensed storagetransportation systems then they could classify the fuel in those systems as nonstandard causing that fuel to lose its place in the DOEs fuel acceptance queue</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Our aim is to strengthen energy markets and encourage innovation throughout the electricity sector giving consumers more choice and greater control over their energy decisions while also benefiting the environment</t>
+          <t>2997 also eliminates the emissions reporting requirement for releases associated with manure under CERCLA Section 103 and Section 304 of EPCRA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>The problem is that if we look ahead and we look at the fact that natural gas is still a fossil fuel comes with CO2 emissions a coaltogas switch will just not be enough to meet our climate goals</t>
+          <t>The reference case includes the effects of several policies aimed at increasing energy efficiency in both enduse technologies and supply technologies including minimum efficiency standards and voluntary energy savings programs</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -698,7 +698,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mr Roberts you mentioned the United Mine Workers in Appalachia and Illinois and I want you to know that there are a lot of them in my district in Western Kentucky and we are excited about Peabody Coal Company being ready to open up a new mine and also entered with a consortium on a power plant also that will use some local coal</t>
+          <t>I guess what I would conclude you said you would not put a roadblock up to exporting coal</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -708,7 +708,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>When they heard about President Obamas proposal to put a tax of 10 on a barrel of American crude oil they all said what the heck what is he thinking</t>
+          <t>FERC grid operators State public utility commissions and power plants even progressive power companies are already planning for the changes that are under way</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -718,7 +718,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I guess what I would conclude you said you would not put a roadblock up to exporting coal</t>
+          <t>We encourage Congress to learn from States like New Mexico when implementing programs to reduce greenhouse gas emissions</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -728,7 +728,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>In fact Congress is in the midst of playing local politics with the most important energy project in the United States</t>
+          <t>A mere requestsomehow provide some assistance so they could be an existing power plant and have beenhave been rebuffed</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -738,7 +738,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>As you will hear today however we believe that elements of the alternative fuels discussion draft as currently constructed will not fully achieve those objectives and may ultimately be counterproductive</t>
+          <t>I believe that we should ask ourselves how Federal investment into clean energy can improve the lives of our constituents and our communities</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -748,7 +748,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>We do have about 9000 megawatts of cogeneration facilities</t>
+          <t>Members of my local union located in Michigan spent months working on the TransAlaska pipeline which covers 800 miles and carries oil from the North Slope of Alaska to Valdez Alaska</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -758,7 +758,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>As members of this committee are well aware FERC has been without a quorum since February which has prevented action on crucial energy infrastructure projects</t>
+          <t>That is the entirety of all of our liabilities that include all of our nuclear ships and the eventual cleanup for those and a variety of other items</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -768,37 +768,37 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>The method can accept a variety of feedstocks including natural gas coal and biomass</t>
+          <t>It goes on to say that the price of coal which fires half of the US power plants has doubled since last year largely because of surging energy use in countries such as China and India</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Well we have already issued a New Source Performance Standard that captures the volatile organic compounds in the emissions from unconventional gas when hydrofracking happens</t>
+          <t>The collateral effects from incomplete or poorly thought out policy changes could have a negative effect on all electricity users and certainly in regions of the country where there are no problems occurring</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Consumers determine energy consumption every day through their purchasing decisions and the use of the products they buy</t>
+          <t>We dont harness the electricity we can from natural gas we dont sell it we dont pull it up we dont benefit the economy from it</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Do you as Commissioner Norris stated the question is not whether we reduce carbon pollution but how and EPA has an answer embodied in the Clean Power Plan and that is what they are proposing as a start</t>
+          <t>In Brazil where a high percentage of ethanol fuels are sold consumers do indeed consider energy content pricing rather than simply buying the cheapest fuel</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -808,7 +808,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>I believe that we should ask ourselves how Federal investment into clean energy can improve the lives of our constituents and our communities</t>
+          <t>The environment doesnt benefit and you have these constricted flows and it seems to me it does not benefit anybody other than the industry that is out there designed to shut down any progress on energy development</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -818,27 +818,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>As Chairman Shimkus stated the 21st Century Transportation Fuel Act Discussion Draft takes a larger view of Federal transportation fuel policies</t>
+          <t>Michael McNulty Attachment B clean power group multiemission control strategy materials Clean Power Groups MultiPollutant Emission Control Strategy The power generation sector is a major contributor to US air pollution</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>It wasnt that long ago that we thought we were out of natural gas as well</t>
+          <t>The USGS has actively participated in two previous Federal reviews of MTBE and other oxygenates in gasoline</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>National and state energy policy can provide for the introduction and demonstration of these other sources so with time they become an integral part of the market</t>
+          <t>NIHtaxpayers paid for it and then smart Wall Street folks bought it and with the benefit of the patent they used that pricing power to overreach</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -848,17 +848,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Remove Market Barriers The first problem we need to solve is a procedural barrier that keeps solar energy from accessing the electricity market</t>
+          <t>I appear this morning on behalf of the National Association of Convenience Stores NACS and the Society of Independent Gasoline Marketers of America SIGMA</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Although more than half the increase in natural gas consumption between 2000 to 2020 is expected in the East the Westincluding Canadian imports and most of the Gulf Offshoreis expected to provide approximately 80 percent of the incremental lower 48 natural gas supply in the reference case</t>
+          <t>And if I can share more expertise that we have in Texas and the south related to wildfire hazardous fuel reduction and prescribed burning</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -868,27 +868,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Have you analyzed how expected and observed climate changes will affect natural gas price fluctuations</t>
+          <t>but our ultimate vision is to establish leadership in hydrogen fuel cells</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>History is on the side of those who want to act on climate change those who believe in the power of American innovation and our ability to successfully meet any challenge and who look to the future rather than the past</t>
+          <t>If not I would ask unanimous consent that wewhen we reconvene at 1030 that opening statementsthe only opening statements we will have will come from the chairman the ranking member of the full committee the chairman and the ranking member of the Energy and Environment Subcommittee</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>So yes I mean I would agree as my testimony alluded to that projects like that in California and other States around the country are being driven in large part by State renewable electricity standards which have been beneficial in not only deploying the technologies but driving down the cost</t>
+          <t>Strong economic growth particularly in China and the United States is fueling a surge in oil demand</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -898,7 +898,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>And then let me ask you when you talked about health and safety of the American folks in looking at the endangerment ruling I am wondering if you all looked at the fact because you mentioned something about the heat being higher causing folks to have strokes or heart attacks etc and I am wondering if you looked at the fact that with the electric rates going up the heating bills going up fuel oil going up that there are a lot of folks in my district who are having a hard time paying for their heat and what is the offset on the other side</t>
+          <t>DOEs newly created Office of Cybersecurity Energy Security and Emergency Response leads these efforts</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -908,7 +908,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>In addition I believe an amendment to the FPA to give the Commission authority to assess penalties in addition to refunds and interest could act as a powerful deterrent against the abuse of market power</t>
+          <t>We are occasionally reminded as we were on August 14th just how significant the loss of electricity can be to our economy and to our daily lives</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -918,7 +918,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Just last month the company was even touted by President Obama for having innovators and creating jobs that will foster our economic recovery and create clean technology to power our longterm prosperity</t>
+          <t>More importantly the draft language does not currently include language that would substantially thwart the Federal Energy Regulatory Commissions FERC current efforts for continued industry restructuring</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -928,17 +928,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>There is an analysis that is going to be released in the coming weeks by the National Commission on Energy Policy</t>
+          <t>The Clean Power Plan I think makes a lot of sense moving forward</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>It took over a year in production and it analyzed all of the various means open to us in terms of investing in energy efficiency technologies</t>
+          <t>Electric cooperatives comprise a unique component of the industry</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -948,7 +948,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>The good news is that almost everything you can imagine as an energy source is also something that can be made to work to produce hydrogen</t>
+          <t>Thus those tax policies stifled the industry at a time when US energy demand was increasing significantly</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -958,7 +958,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>We doare very interested as I said in my remarks want to see the full investigation because we want to understand was there something else people were looking at that caused them to make the decisions they made as opposed to making the decisions that almost any of our drilling operations people would have made differently that led to the ultimate loss of the well</t>
+          <t>I joined the Department of Energy back in 1978 and I joined the program in 1985</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -968,17 +968,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>CAFE standards have helped increase the average fuel economy of our lightduty vehicle fleet</t>
+          <t>Have you analyzed how expected and observed climate changes will affect natural gas price fluctuations</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>In their wisdom the founders of our Nation gave Congress the constitutional power to protect the Intellectual Property of Authors and Inventors in order to promote the Progress of Science and the useful Arts</t>
+          <t>This one is from TXU Energy down in Texas</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -988,7 +988,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Siemens Ford and Volvo have all made engines that reduce particulate emissions by more than 90 percent and nitric oxides similarly remarkably reduced</t>
+          <t>Consumers determine energy consumption every day through their purchasing decisions and the use of the products they buy</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -998,17 +998,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>bullet First we need a strong and sustained push from Congress and the Administration to support biofuel production including nextgeneration cellulosic ethanol</t>
+          <t>I look forward to todays hearing to examine the challenges and opportunities to modernize our electric grid</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>We dont add carbon monoxide to make product look fresh beyond its code date</t>
+          <t>Nuclear science and technologies take advantage of radiation and nuclear properties of the atom to perform many useful activities such as improving food safety protecting our homeland and providing for precise industrial production</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1018,17 +1018,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>For example for an average family driving 2500 miles a month a 1 gallon runup in gasoline prices as we have seen in recent weeks takes 120 out of their monthly budget if they are driving vehicles that average 21 miles per gallon but it would only take 60 out of their budget if those vehicles average 42 miles per gallon which is within our technical capability</t>
+          <t>However the US Congress does possess the power to overturn some of the most important barriers facing Distributed Generation today</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Four US States Minnesota Montana Idaho and North Dakota account for 75 percent of all the natural gas brought into the United States via pipeline</t>
+          <t>In addition TIGR has also sequenced a wide range of important environmental microbessome of which live in extreme environments but may be critically important to the health of the planetand that carry out a variety of interesting metabolic reactions including degradation of cellulose and other organic matter precipitation of heavy metals such as uranium from solution and production of methane and hydrogen as potential new sources of fuel</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1038,7 +1038,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>They have no electricity</t>
+          <t>Public power also sells any excess power when available in the wholesale market</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1048,27 +1048,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Shifting gears I believe the Energy Star program is a nice complement to the mandatory federal energy efficiency standards for many energyusing products in that it helps consumers identify those models that go above and beyond the minimum standards</t>
+          <t>Could we talk for just a minute about the energy policy that is being followed by this administration</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>The commission has a stake in the national energy policy and has identified areas where new legislation would be helpful</t>
+          <t>Again less American jobs more dependence on foreign oil</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>One of the technologies we are currently applying alongside of the SAGD is cogeneration a very energyefficient process that produces both steam for our operations and electricity for the sale to the grid</t>
+          <t>As you all know the first export of LNG to scheduled to happen later this month maybe early March at Sabine Pass in Louisiana right next to Texas my own State</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1078,17 +1078,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>And many of the coops in my district have supported an alloftheabove energy policy</t>
+          <t>This initiative requires relatively modest federal investment in nuclear energy research and development</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Well let me just ask you this then are you basing determinations on LNG exports in part on those discussions with the G7 nations</t>
+          <t>The prepared statement of Jerry Jordan follows Jerry Jordan on Behalf of the Independent Petroleum Association of America and the National Stripper Well Association 1 1 Colorado Oil Gas Association East Texas Producers Royalty Owners Association Eastern Kansas Oil Gas Association Florida Independent Petroleum Association Illinois Oil Gas Association Independent Oil Gas Association of New York Independent Oil Gas Association of Pennsylvania Independent Oil Gas Association of West Virginia Independent Oil Producers Association TriState Independent Petroleum Association of Mountain States Independent Petroleum Association of New Mexico Indiana Oil Gas Association Kansas Independent Oil Gas Association Kentucky Oil Gas Association Louisiana Independent Oil Gas Association Michigan Oil Gas Association Mississippi Independent Producers Royalty Association Montana Oil Gas Association National Association of Royalty Owners Nebraska Independent Oil Gas Association New Mexico Oil Gas Association New York State Oil Producers Association Ohio Oil Gas Association Oklahoma Independent Petroleum Association Panhandle Producers Royalty Owners Association Pennsylvania Oil Gas Association Permian Basin Petroleum Association Tennessee Oil Gas Association Texas Alliance of Energy Producers Texas Independent Producers and Royalty Owners and Wyoming Independent Producers Association</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1098,17 +1098,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Our objectives area to exercise and perform the powers and duties assigned to the IMO under this Act the market rules and its licenceb enter into agreements with transmitters giving the IMO authority to direct the operations of their transmission systemsc direct the operations and maintain the reliability of the IMO controlled gridd establish and operate the IMOadministered marketse collect and provide to the public information relating to the current and future electricity needs of Ontario and the capacity of the integrated power system to meet those needsf participate in the development by any standards authority of standards and criteria relating to the reliability of transmissions systems andg work with responsible authorities outside Ontario to coordinate the IMOs activities with their activities</t>
+          <t>And there have been a few sites like in Monroe Michigan where there is actually an assembly plant for wind energy</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>She thought everybody had asthma because they are all breathing that diesel smoke and toxic fumes</t>
+          <t>Today Big Oil and Big Coal have been working with the Republican thought police to comb through each and every reference to global warming pollution in the Clean Air Act and then disappear them sending scientific consensus down the memory hole at the expense of public health and welfare</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1118,7 +1118,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>These are just a few of the growing costs of carbon pollution</t>
+          <t>For the first time in six decades the United States is a net natural gas exporter</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1128,17 +1128,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Electric utilities also have a long history of providing mutual assistance and the same concept is being applied by the ESCC for mutual support in response to cyber incidents though challenges unique to cyber must be taken into account</t>
+          <t>In recent years we have seen the impact of relying almost exclusively on natural gas based plants for new generation tight gas supply higher prices and backlogged projects for natural gas based plants</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>We need metals for our legacy energy businesses our carbonbased businesses oil gas coal whatever</t>
+          <t>The proposal would require all generators public utilities and power marketers to file electronically with the Commission and post on the Internet an index of customers with a summary of the contractual terms and conditions for marketbased power sales costbased power sales and transmission service</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1148,27 +1148,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>If thats the case for a State like Illinois if 40 percent of the power that we generate is nuclear what would that do to our national energy policy and the pocketbook issues what would it do to the price for the individual consumers</t>
+          <t>The Report notes that The energy burden on lowincome households as a proportion of income is four times greater than for other American households</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>OK Do pollution controls affect the power plants energy efficiency</t>
+          <t>So for instance one of my companies Sun Drop Fuels has adopted a different model so they went to Chesapeake a natural gas company because they are going to use natural gas as part of the feedstock in their plant</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Americas hydrocarbon renaissance has given us the gift of time</t>
+          <t>Coalfired electricity is only cheap if one ignores the health and economic costs</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1178,17 +1178,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Second EPA is about to begin an emissions trading program for nitrogen oxide in the northeast and midwest which will also bring about significant reductions beginning in 2003</t>
+          <t>But you continue to hide evaporative emissions by even using tailpipe emissions in my opinion</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>The other waiver authority which you referenced is a general waiver authority where if the administrator can either be petitioned by a party or can on her own determine that the RFS implementation would create a severe economic harm to a region or a State and that the previous conversation we have been petitioned a couple of times and determined that again because of market dynamics and the demand that the refining industry has for ethanol that the statutory test simply was not met and we are not allowed to grant that waiver</t>
+          <t>While the blackout was a singular unprecedented event the fact remains that our national electric transmission system needs significant improvement and that we need to continue our efforts to enhance system reliability by expanding and improving the transmission system capabilities and interconnections</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1198,7 +1198,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>I am president and CEO of Southwest Power Pool an organization for which I have worked 32 years</t>
+          <t>Such macroeconomic conditions generally present from the 1930s to the 1980s maintained low electricity rates and reliable service for end customers while strong predictable returns for investors</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1208,27 +1208,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>As you all know the first export of LNG to scheduled to happen later this month maybe early March at Sabine Pass in Louisiana right next to Texas my own State</t>
+          <t>The savings from the CAFE proposal like I mentioned is more than three times proven reserves of oil in the United States</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Today we will hear from the Federal Energy Regulatory Commission which is the coordinating agency for these reviews</t>
+          <t>Dr Ebinger paints a very positive picture resulting from lifting the crude oil export ban reporting a gain in GDP over the next 25 years of 600 billion orbillion to 18 trillion</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>We see this in the programs that have received proposed budget increases like the 29 billion for the Office of Energy Efficiency and Renewable Energy a 40 percent increase</t>
+          <t>Congressman if you dont mind I think I will jump into this first and I would ask maybe to submit for the record the most recent comprehensive study conducted by the Department of Energys Argonne National Lab which looked at all of the energy balance studies that have been done over the past 10 and 15 years and concluded that without question ethanol has a positive energy balance</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1238,7 +1238,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>The fuel diversity should be a cornerstone of our national energy policy as an important hedge against supply disruptions and price volatility</t>
+          <t>A 10 percent reduction in environmental management an 8 percent reduction in the Office of Science 86 percent reduction in energy efficiency and renewable energy</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1248,37 +1248,37 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>What we also do is allow forwhat the legislation does it allow for technology limits 60 percent I think to one technology 90 percent for two and what that is doing there is saying that although wind today is the cheapest form of renewable power generation ultimately because of these cost curves you want to induce more competition and to see oil prices continue to come down</t>
+          <t>We see Wisconsins electricity demand growing by almost 3 percent per year</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>I have been downstairs at the hearing on subsidies and price gouging on gas prices and we will be bouncing back and forth all day</t>
+          <t>Im frustrated that the Bush administration is decimating important R D programs and not establishing realistic and attainable goals for our energy future</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Through research and demonstration of hydrogen generation and storage technology we will be able to gain the necessary safety knowledge which will lead to data driven codes and standards that do not currently exist</t>
+          <t>The Johnson Johnson 7 Minute Wellness for Expecting and New Moms App is a sciencebased wellness resource designed to help new moms manage and expand their energy during pregnancy and after giving birth</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>but our ultimate vision is to establish leadership in hydrogen fuel cells</t>
+          <t>Instead as the threat from climate change becomes more and more dire and the scientific consensus of the threat becomes even clearer we are having another hearing focused on the alleged war on coal</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1288,47 +1288,47 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>While that is a viable use for injected carbon we also need to store large quantities of it underground indefinitely and on that front further research development and demonstration is clearly called for</t>
+          <t>She thought everybody had asthma because they are all breathing that diesel smoke and toxic fumes</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>FERCs authority to review proposed mergers should be expanded to include mergers of holding companies transfers of generation facilities and consolidation of electric and natural gas companies</t>
+          <t>Texas Pacific and Kohlberg Kravis Roberts the famous KKR purchased Texas Utility Corporation and agreed to terminate 8 of 11 proposed coalfired power plants</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>That was in my energy business</t>
+          <t>We have a very favorable climate for construction approval siting of new power plants new generating facilities</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>It can also help ensure that our communities are more resilient to the impacts of climate change as you know well in your State from power outages to flooding and storm surges</t>
+          <t>My advice to you would be that there would be incentives for the continued investment and development of technology to reduce carbon which does not yet exist</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>And there have been a few sites like in Monroe Michigan where there is actually an assembly plant for wind energy</t>
+          <t>The commission has a stake in the national energy policy and has identified areas where new legislation would be helpful</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1338,17 +1338,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>If not I would ask unanimous consent that wewhen we reconvene at 1030 that opening statementsthe only opening statements we will have will come from the chairman the ranking member of the full committee the chairman and the ranking member of the Energy and Environment Subcommittee</t>
+          <t>But for the sake of our consumers our utility businesses and Americas entrepreneurs and innovators we as a Nation could take a better course of action and enact a national energy policy to begin the transition to a lowcarbon economy</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>What type of an impact would meeting the goals of the Renewable Fuel Standard have on jobs here in America</t>
+          <t>Are you both familiar with the EPAs efforts and have you been invited at all to participate in their process of establishing a registry and if so could you elaborate on some of the suggestions that you have made to design a registry and recognizing of course that we already are doing emissions registry in the electrical sector</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -1358,37 +1358,37 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Up to 4000 megawatts of capacity nationwide would be eligible</t>
+          <t>It wasnt that long ago that we thought we were out of natural gas as well</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>I mean I dont want to be an expert in gas cans to be able to use that product</t>
+          <t>I know their program is what they are trying to develop there is also been using solar panels so they can go to areas without electricity and still be able to process water for families in that immediate area</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>For example the Chairman of the Crow Nation the tribal Nation in Montana has testified before congress that the importance of coal mining to the economy of the Crow Reservation cannot be overstated</t>
+          <t>You do have on the website a page and email address to accept public comments and requests regarding the Federal Power Act section 202 but I just want to make sure that they will be posted for the public to see</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>The principal environmental benefits associated with coal gasification as compared to coal combustion processes are in the short term significantly lower emissions of serious air pollutants such as sulfur dioxide NOINFXINF and I should say almost virtual removal of volatile mercury</t>
+          <t>First it is the tax subsidies for unconventional energy that by far have the most detrimental effects on markets prices and consumers</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -1398,7 +1398,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>However while we look forward to advanced nuclear technology development it is long overdue to solve our Nations nuclear waste disposal challenge</t>
+          <t>As states get closer to the implementation date for their fuel programs the greater the temptation to change the date rather than deal with the uncertainty</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -1408,27 +1408,27 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Michael McNulty Attachment B clean power group multiemission control strategy materials Clean Power Groups MultiPollutant Emission Control Strategy The power generation sector is a major contributor to US air pollution</t>
+          <t>No market participant in interstate wholesale electric markets should be immune from FERCs investigative and remedial authority</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>I am privileged to chair the Subcommittee on Commerce Trade and Consumer Protection and my friend and colleague Mr Boucher who is the chairman of the Communications Technology and Internet Subcommittee of the Committee on Energy and Commerce</t>
+          <t>Towns which adds some common sense to a currently onerous relicensing process for nonfor Federal hydro projects</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>In this same vein expert witnesses are called before us today to discuss policies to deeply decarbonize our economy and strengthen our infrastructure against threats like climate change</t>
+          <t>The Commission has been upheld in its interpretation of the Federal Power Act as excluding generation facilities per se from our direct authority</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -1438,10 +1438,1010 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>AGA represents 185 local natural gas distribution companies which deliver natural gas to 50 million customers in the United States</t>
+          <t>This authority is vested in the Secretary of Energy and has been delegated to the assistant secretary for fossil energy</t>
         </is>
       </c>
       <c r="B101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Should this final FIP result in closure of the San Juan plant and mine hundreds of jobs will be lost not only in the coal and power industry on the Nation but in the service support industry and public sector as well</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>The electricity cost in 2020 under the LiebermanWarner Bill was 28 to 33 percent increase and in 2030 101 percent to 129 percent</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>And Mr Shimkus is from a State that has the most spent nuclear waste in the country</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>As Ohioans discuss this issue across the state we hear one overriding concern maintaining our affordable reliable power is critical to both the pocketbooks of Ohioans and continued economic development within our state</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Do you as Commissioner Norris stated the question is not whether we reduce carbon pollution but how and EPA has an answer embodied in the Clean Power Plan and that is what they are proposing as a start</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>In some conversations that I have had with individuals concerned about some smaller engines those in boats or motorcycles and other specialty vehicles they have had trouble running on even blends with 10 percent ethanol</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>You would be a real hero if you could get us the energy bill</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Power supplies had been disabled</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>This further diminishes their bargaining power because it is now an emergency</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>This added step of accountability is crucial to keep an account of delays and avoid the increasing backlog of hydropower relicensing</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Soand the other thing I would add is that they are not clean or completely fossilfuel free the way that renewables are</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>These are good solid domestic jobs that get created with energy efficiency</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>The wood products industry is a leading user of wood fiber and producer and user of carbonneutral renewable biomass energy to run our plants</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Last fall we published a report Biofuels Issues and Trendsit is attached to my testimonyto provide an overview of the dynamics of production consumption trade in ethanol biodiesel and cellulosic fuels</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Id like to talk about one thing that largely did work and thats nuclear energy</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>As the FERC commissioners make clear in their letter a thorough assessment of the impacts of for example the proposed Clean Power Plan requires the ongoing input of diverse perspectives and expertise</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Not only steel producers chemical plants or power plants are taking part in this trading also banks and insurances making this really a vivid trading place</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>You noted at the outset of your tenure at the EPA that your goal was to refocus EPA on its intended mission return power to the states and create an environment where jobs can grow</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>So therefore the regional power market does not see the price signal that RGGI is intended to deliver</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Mercury that ends up in fish may originate as emissions to the air</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Instead what weve learned from a steady stream of press reports and congressional hearings is that bullet EPA in fact concluded that greenhouse gas emissions endanger public welfare and submitted its finding to OMB in December of last year</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>This bill is a radical rewrite of the Clean Air Act that would block any real reductions in carbon pollution from coal plants and it ignores 40 years of experience</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Is that enough reliance or should we do modeling before we resume exploration and drilling in the Gulf of Mexico</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>The fact remains it was under Secretary Salazar that BPs initial exploration plan was reviewed and approved by the Minerals Management Service</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>So this slide shows how you would replace one nuclear reactor that is 1154 megawatts with wind</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>We had better find a way to use coal in a clean manner</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Technological advancements on the electrical grid from transmission through end use have helped improve efficiency and reduced emissions</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>And the clean energy sector employed roughly three times more workers than the fossil fuel sector in 2019</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Second the National Nuclear Security Administrations direct Federal oversight was narrowly focused on specific performance measures called out in the contract rather than on overall effectiveness and the interface between different areas and I will say more about this in a moment</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>The United States has such incredible energy abundance</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>I think the natural markets that have formed that have some reasonable transmission capability within that region so you can move significant amounts of power within that region is a good start</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>It goes actually to the heart of what I have talked about which is when you look at energy independence and we look at developing as part of a national security strategy and having an energy policy when you look at those refineries and 30 percent being owned by foreign interests when you look at 30 percent of our oil or 27 being imported into the United States if you want to look at it at a freemarket perspective we dont have a free market</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Mr Linn and Mr Duplessis obviously with this being the largest oil spill in the history of our country theres lots of media attention</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Dynegy owns or controls approximately 14000 megawatts of generating capacity in the United States of which 2750 is in California</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>It is the agency that makes sure your coffee maker does not burn down your house your baby does not die from a defective crib your power drill doesnt electrocute you your hot water heater does not poison you your childs toy is not made of lead et cetera and these are all real examples of defective products that have been recalled and they demonstrate the important role the Commission should play in protecting consumers</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>1013 would create more red tape and delay and would severely reduce protections for rivers and fisheries impacted by hydroelectric generation</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>This bill sets out a national strategy to assist US clean energy technology companies with export assistance to find new markets for their products and services and to better compete in the international marketplace</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Were you involved in any communications with the White House to push the Department of Energy to speed this thing along</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>I think essential to the Yucca Mountain project to store the spent fuel down there would be a rail line</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>But I worry that you will labor mightily and give forth with a capandtrade that will produce a carbon price that is too low to affect physical change</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>The company also engages in new hydropower development through the building of new plants at existing dams</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>As Member of Congress from East Harris County and Houston Texas I have just literally hundreds of people who work offshore offshore Texas offshore literally all over the world and along with our infrastructure we still produce oil and natural gas in a very urbansuburban area but we also have refineries and chemical plants who need that product that is being produced</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>It is the utilities driving renewable growth and many other independent power producers driving renewable growth and we can take advantage of those independent power producers through very competitive RFPs and PPAs and certainly with our own facilities</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Through research and demonstration of hydrogen generation and storage technology we will be able to gain the necessary safety knowledge which will lead to data driven codes and standards that do not currently exist</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Technology can also be a driver for increased energy efficiency and Reps McNerney Welch and Kinzinger have introduced bills that analyze and support new technologies in smart buildings and water systems</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Im surprised Mr Garman didnt sort of agree with what I told him about petroleum</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>A key responsibility of this Committee is to develop and ensure implementation of a Strategic Plan for disposition and consolidation of special nuclear material</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>And in fact even as we speak here this afternoon officials in Louisiana are still waitingstill waiting for the Federal Government to provide millions of feet in boom to approve an emergency permit to fullynot partiallyimplement their plan to dredge and build a new barrier island to prevent even more oil from reaching their marshes and wetlands</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>There are a lot of options available to us in the short and long term to produce hydrogen from a variety of different sources and thats one of its attractions</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>And then we have Mr Lou Pugliaresi who is the president of Energy Policy Research Foundation</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>So I would just ask that you go and pursue the administration policies that are killing energy production and causing higher gas prices instead of going to Saudi Arabia</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Hydro provides six to seven percent of all electricity generation and nearly half of all renewable generation making hydro the largest provider of renewable electricity</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>And then let me ask you when you talked about health and safety of the American folks in looking at the endangerment ruling I am wondering if you all looked at the fact because you mentioned something about the heat being higher causing folks to have strokes or heart attacks etc and I am wondering if you looked at the fact that with the electric rates going up the heating bills going up fuel oil going up that there are a lot of folks in my district who are having a hard time paying for their heat and what is the offset on the other side</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>NNSA is responsible for overseeing the approval while consulting the Office of Nuclear Energy and the DOE general counsel in addition to interagency coordination</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Do you think that all drinking water systems that are located near wastewater treatment facilities that accept drilling waste should monitor intake water for radioactivity and other potentially hazardous byproducts of these activities</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Question 3 How does the new supply margin market power test in the Commissions order of November 20 differ from the established hubandspoke test for market power</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>But in fact I think it has worked out very well in the electric sector in the sense that we have utilities all other extensions above power systems or at least meeting minimum standards and we saw a good example with Texas this past winter</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>A special report of the Institutes oxygenates evaluation committee Cambridge MA Health Effects Institute April 1996 httpwwwhealtheffectsorgPubsoxysumhtm National Institute of Environmental Health Sciences 2002 MTBE in gasoline National Institute of Environmental Health Sciences March 13 2002 httpwwwniehsnihgovexternalfaqgashtm SUP13SUP Toccalino supra citing inter alia National Science and Technology Council 1996 Interagency assessment of potential health risks associated with oxygenated gasoline Washington DC National Science and Technology Council Committee on Environment and Natural Resources February 1996 httpwwwostpgovNSTChtmlMTBEmtbetophtml Office of Science and Technology Policy 1997 Interagency assessment of oxygenated fuels Washington DC Office of Science and Technology Policy National Science and Technology Council Executive Office of the President of the United States June 1997 264 p httpwwwepagovomsregsfuelsostpfinpdf U S Environmental Protection Agency 1997 Drinking water advisory Consumer acceptability advice and health effects analysis on methyl tertiarybutyl ether MTBE Washington DC U S Environmental Protection Agency Office of Water EPA822F97009 December 1997 48 p httpwwwepagovwatersciencedrinkingmtbepdf</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Do you agree or disagree that it is too late to prevent the carbon dioxide emissions from increasing to 450</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Although more than half the increase in natural gas consumption between 2000 to 2020 is expected in the East the Westincluding Canadian imports and most of the Gulf Offshoreis expected to provide approximately 80 percent of the incremental lower 48 natural gas supply in the reference case</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Reprogramming by nuclear transfer is faster than genebased reprogramming and may entail very different mechanisms that will teach us a lot about how to make pluripotent tissues better</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>These types of facilitiesexempt wholesale generators or EWGsare not considered to be electric utility companies under PUHCA and in fact are exempt from all provisions of PUHCA</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>In terms of the policies of Alberta there are policies in place to recognize that the upfront costs of developing oil sands are very very high</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Some are reliably available 24 hours a day and seven days a week and ideal for baseload power while others are not</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Secondly the other consistent thing in that report as I stated earlier is the natural gas impact is having on the marketplace in general in terms of retiring old inefficient plants</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>We do have about 9000 megawatts of cogeneration facilities</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>So if that were correct and I dont disagree with you on that coming from a coal State but if that is correct then why are we having policy that is moving us in that direction</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>When that merging occurs will we on the Energy and Commerce Committee be made aware of what that structure looks like and how the fund then subsequently is to be administered</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Todays hearing is surfacing some concerns about the power platforms have to editorialize the things internet users read and say but at the same time the FCC is considering wholesale elimination of rules that prevent broadband providers from doing that</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>The prepared statement of Glenn English follows Glenn English Chief Executive Officer National Rural Electric Cooperative Association INTRODUCTION Chairman Barton and Members of the Subcommittee I appreciate this opportunity to continue our dialogue on the restructuring of the electric utility industry</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Certainly methane capture from landfills is fairly easy to measure</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>As you will hear today however we believe that elements of the alternative fuels discussion draft as currently constructed will not fully achieve those objectives and may ultimately be counterproductive</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Shifting gears I believe the Energy Star program is a nice complement to the mandatory federal energy efficiency standards for many energyusing products in that it helps consumers identify those models that go above and beyond the minimum standards</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>You guys are the guys who can make this happen because of your connection with mostlyyou have some friends over on my side but you have a lot of friends on the Democrat side and they are in charge and so I would plead with you and the other folks who are looking for expansion of energy opportunities the operating engineers the electricians that they hold out for a good bill that they are not going to lose their jobs</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>OK Do pollution controls affect the power plants energy efficiency</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Well I am just in the research and analysis business but I would thinkand my friends in the industry can speak perhaps better but I think the biggest concern or two really one would be that the government is going to stand in the way of infrastructure projects that are needed to get investment in domestic oil and gas production and the second would be uncertainty about regulation of hydraulic fracturing going forward</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>And you need to understand how they function and just going in and building a tighter envelopethis happened when I was a code official back in the early 90s is the energy code started requiring tighter construction</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Under the Federal Power Act the Federal Energy Regulatory Commission known as FERC oversees electricity markets and the physical and virtual products traded within them</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Well from a fire science perspective you always have to remember you have to have drying of the fuels to a point where they can be ignited and sustain ignition and you have to have ignition</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Diesel trucks are paying 450 a gallon for diesel</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>I was sitting here listening thinking of a hearing we had not many weeks ago and Mr Greenspan was with us talking about the current situation with natural gas supplies and pricing in this country</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Environmental concerns are extremely important because energy production and consumption involve major externalitiescosts that are not easily reflected in market transactions</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>This will result in higherthannormal gas commodity prices even if the winter is relatively mild</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>And the bulkpower system includes facilities and control systems necessary for operating an interconnected electric energy transmission network</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Renewable fuel standard is putting 36 billion gallons of nongasoline into the gasoline and diesel supply through the next few decades</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Sometimes we will give them energy sometimes they will give us energy</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>The future will belong to the country that builds an energy infrastructure to support a cleaner low carbon economy</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>We may even get some pleasant surprises such as we recently experienced with the shale gas revolution</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>In another example we believe US EPA has misapplied the economic feasibility analysis to predict the reliability on the bulk power system</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>For illustrative purposes 43 quads is equivalent tobullet Over 20 million short tons of coal or enough coal to fill a coal train of railroad cars almost 2000 miles longbullet 418 billion cubic feet of natural gasbullet Almost 35 billion gallons of gasoline or more than 10 days of US gasoline consumptionbullet Almost 10 hours of the entire worlds energy use based on consumption levels in 1996bullet Nearly half of the approximate annual primary consumption of any one of the following states Arizona Arkansas Colorado Iowa Kansas Mississippi or Oregon based on consumption levels in 1996 This 43 quads represents a 39 total annual savings in cooling and a 19 savings in heating or a total heat and cooling savings of approximately 25 billion per year by 2010 given an adoption baseline of 1996</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>And the second is that Congress has power to substantially correct it if it so chooses</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>This work to better organize the healthcare market into highvalue networks is necessary and desirable and we would urge that folks make a differentiation between consolidation to create excessive market power and integration of providers in the market to create a highvalue network</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>The C2P2 encourages generators and users of coal combustion products to increase the use of coal ash in cement and other construction products</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>For example advanced nuclear technologies might be one thing that you could put into repower an existing fossil generating plant like that</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Well just to add on that most of the nuclear plant sites in the country have had to add additional storage capacity either in the form of expanding the pools themselves or how to manage the pools or putting them in what is known as dry cask storage</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>We have Mr Adam Sieminski Chief Energy Economist Deutsche Bank</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>This need not be limited to natural gas or other energy products</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>What do you see as the Federal Governments proper role in encouraging the use of alternative fuels in vehicles</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>We are still overly dependent on foreign oil from countries that clearly we have seen especially over the last 15 years do not represent our interests and values</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>The National Academy of Sciences has referred to the US electricity grid as the greatest engineering achievement of the 20th century because it delivers critical energy services to consumers in an instantaneous affordable and dependable manner</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>